<commit_message>
Quote status working for adding and deleting.
</commit_message>
<xml_diff>
--- a/drafts/CRM-schema.xlsx
+++ b/drafts/CRM-schema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Field Names" sheetId="1" r:id="rId1"/>
@@ -580,7 +580,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">cars = ["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"] </t>
+    <t>["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],</t>
   </si>
 </sst>
 </file>
@@ -698,7 +698,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="241">
+  <cellStyleXfs count="256">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -831,6 +831,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -976,7 +991,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="241">
+  <cellStyles count="256">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1151,6 +1166,21 @@
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1551,7 +1581,7 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -2076,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X48"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3085,7 +3115,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="76">
+    <row r="15" spans="1:24" ht="121">
       <c r="A15" s="11" t="s">
         <v>106</v>
       </c>
@@ -3093,19 +3123,19 @@
         <v>154</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>86</v>
+        <v>154</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>82</v>
+        <v>154</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>85</v>
@@ -3652,138 +3682,6 @@
       </c>
       <c r="W22" s="2" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" ht="16">
-      <c r="B27" t="str">
-        <f>'Document Data'!$A$1</f>
-        <v>coll.insert({</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" ht="16">
-      <c r="B28" t="str">
-        <f>CONCATENATE('Document Data'!$A28,"'",'Document Data'!C28,"',")</f>
-        <v>'',</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" ht="16">
-      <c r="B29" t="str">
-        <f>CONCATENATE('Document Data'!$A29,'Document Data'!C29)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:23" ht="16">
-      <c r="B30" t="str">
-        <f>CONCATENATE('Document Data'!$A30,'Document Data'!C30)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="16">
-      <c r="B31" t="str">
-        <f>CONCATENATE('Document Data'!$A31,'Document Data'!C31)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:23" ht="16">
-      <c r="B32" t="str">
-        <f>CONCATENATE('Document Data'!$A32,'Document Data'!C32)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="2:2" ht="16">
-      <c r="B33" t="str">
-        <f>CONCATENATE('Document Data'!$A33,'Document Data'!C33)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="2:2" ht="16">
-      <c r="B34" t="str">
-        <f>CONCATENATE('Document Data'!$A34,'Document Data'!C34)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="2:2" ht="16">
-      <c r="B35" t="str">
-        <f>CONCATENATE('Document Data'!$A35,'Document Data'!C35)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="2:2" ht="16">
-      <c r="B36" t="str">
-        <f>CONCATENATE('Document Data'!$A36,'Document Data'!C36)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="2:2" ht="16">
-      <c r="B37" t="str">
-        <f>CONCATENATE('Document Data'!$A37,'Document Data'!C37)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="2:2" ht="16">
-      <c r="B38" t="str">
-        <f>CONCATENATE('Document Data'!$A38,'Document Data'!C38)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="2:2" ht="16">
-      <c r="B39" t="str">
-        <f>CONCATENATE('Document Data'!$A39,'Document Data'!C39)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="2:2" ht="16">
-      <c r="B40" t="str">
-        <f>CONCATENATE('Document Data'!$A40,'Document Data'!C40)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="2:2" ht="16">
-      <c r="B41" t="str">
-        <f>CONCATENATE('Document Data'!$A41,'Document Data'!C41)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="2:2" ht="16">
-      <c r="B42" t="str">
-        <f>CONCATENATE('Document Data'!$A42,'Document Data'!C42)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="2:2" ht="16">
-      <c r="B43" t="str">
-        <f>CONCATENATE('Document Data'!$A43,'Document Data'!C43)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="2:2" ht="16">
-      <c r="B44" t="str">
-        <f>CONCATENATE('Document Data'!$A44,'Document Data'!C44)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="2:2" ht="16">
-      <c r="B45" t="str">
-        <f>CONCATENATE('Document Data'!$A45,'Document Data'!C45)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="2:2" ht="16">
-      <c r="B46" t="str">
-        <f>CONCATENATE('Document Data'!$A46,'Document Data'!C46)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="2:2" ht="16">
-      <c r="B47" t="str">
-        <f>CONCATENATE('Document Data'!$A47,'Document Data'!C47)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="2:2" ht="16">
-      <c r="B48">
-        <f>'Document Data'!E48</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3815,8 +3713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="E9" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="66.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5084,27 +4982,27 @@
     <row r="15" spans="1:22">
       <c r="A15" t="str">
         <f>CONCATENATE('Document Data'!$A15,'Document Data'!B15)</f>
-        <v xml:space="preserve">tech:cars = ["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"] </v>
+        <v>tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],</v>
       </c>
       <c r="B15" t="str">
         <f>CONCATENATE('Document Data'!$A15,'Document Data'!C15)</f>
-        <v>tech:'Django',</v>
+        <v>tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],</v>
       </c>
       <c r="C15" t="str">
         <f>CONCATENATE('Document Data'!$A15,'Document Data'!D15)</f>
-        <v>tech:'NoSQL',</v>
+        <v>tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],</v>
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE('Document Data'!$A15,'Document Data'!E15)</f>
-        <v>tech:'JavaScript',</v>
+        <v>tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],</v>
       </c>
       <c r="E15" t="str">
         <f>CONCATENATE('Document Data'!$A15,'Document Data'!F15)</f>
-        <v>tech:'HTML5',</v>
+        <v>tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],</v>
       </c>
       <c r="F15" t="str">
         <f>CONCATENATE('Document Data'!$A15,'Document Data'!G15)</f>
-        <v>tech:'SQL',</v>
+        <v>tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],</v>
       </c>
       <c r="G15" t="str">
         <f>CONCATENATE('Document Data'!$A15,'Document Data'!H15)</f>
@@ -5804,7 +5702,31 @@
     <row r="27" spans="1:22" ht="272" customHeight="1">
       <c r="A27" s="13" t="str">
         <f>CONCATENATE(A1,A2,A3,A4,A5,A6,A7,A8,A9,A10,A11,A12,A13,A14,A15,A16,A17,A18,A19,A20,A21,A22)</f>
-        <v>coll.insert({quoteId:' "1",',name: "Mr. Simpson",email: "ciaran.quinlan@gmail.com",phone: "0868090777",rankQuality: "Low",rankTime: "Medium",rankCost: "High",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "4000",brief: "Becoming a fullstack web developer requires you to cover a lot of skills. For beginners it’s often not easy to find the right learning path and to gain quick result. At first sight it might be overwhelming to understand what you need to learn and how everything fits together at the end..",typeDev:'Responsive Web Development (HTML5/JSON/REST)',tech:cars = ["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"] quoteStatus: "open",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:' "1",',name: "Mr. Simpson",email: "ciaran.quinlan@gmail.com",phone: "0868090777",rankQuality: "Low",rankTime: "Medium",rankCost: "High",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "4000",brief: "Becoming a fullstack web developer requires you to cover a lot of skills. For beginners it’s often not easy to find the right learning path and to gain quick result. At first sight it might be overwhelming to understand what you need to learn and how everything fits together at the end..",typeDev:'Responsive Web Development (HTML5/JSON/REST)',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "open",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+      </c>
+      <c r="B27" s="13" t="str">
+        <f>CONCATENATE(B1,B2,B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19,B20,B21,B22)</f>
+        <v>coll.insert({quoteId:' "2",',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime:"Low",rankCost: "Medium",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "5000",brief: "Becoming a fullstack web developer requires you to cover a lot of skills. For beginners it’s often not easy to find the right learning path and to gain quick result. At first sight it might be overwhelming to understand what you need to learn and how everything fits together at the end..",typeDev:'Native Mobile Application (iOS)',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "closed",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+      </c>
+      <c r="C27" s="13" t="str">
+        <f t="shared" ref="C27:G27" si="0">CONCATENATE(C1,C2,C3,C4,C5,C6,C7,C8,C9,C10,C11,C12,C13,C14,C15,C16,C17,C18,C19,C20,C21,C22)</f>
+        <v>coll.insert({quoteId:' "3",',name: "Mr. Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "High",rankTime: "Medium",rankCost:"Low",levelQuality:"Jumbo Jet",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This post will give you an overview of technologies you may consider to learn for being a fullstack developer in 2019 and beyond. We’ll start to take a look at the foundation and programming languages and then move forward to more advanced topics like frameworks and additional tools..",typeDev:'E-Commerce Web Development',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "pending",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+      </c>
+      <c r="D27" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>coll.insert({quoteId:' "4",',name: "ciaran",email:"random@email.com",phone: "0868090777",rankQuality:  "High",rankTime: "High",rankCost: "Medium",levelQuality:"Space Shuttle",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "4000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Database Architecture and Design',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "open",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+      </c>
+      <c r="E27" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>coll.insert({quoteId:' "5",',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality: "Low",rankTime: "Medium",rankCost: "High",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "5000",brief: "this is the detailed brief",typeDev:'Bespoke Software Platform',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "closed",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+      </c>
+      <c r="F27" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>coll.insert({quoteId:' "6",',name: "Mr. Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime:"Low",rankCost: "Medium",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "Becoming a fullstack web developer requires you to cover a lot of skills. For beginners it’s often not easy to find the right learning path and to gain quick result. At first sight it might be overwhelming to understand what you need to learn and how everything fits together at the end..",typeDev:'Other:',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "pending",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+      </c>
+      <c r="G27" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>coll.insert({quoteId:' "7",',name: "ciaran",email:"random@email.com",phone: "0868090777",rankQuality:  "High",rankTime: "Medium",rankCost:"Low",levelQuality:"Jumbo Jet",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "4000",brief: "This post will give you an overview of technologies you may consider to learn for being a fullstack developer in 2019 and beyond. We’ll start to take a look at the foundation and programming languages and then move forward to more advanced topics like frameworks and additional tools..",typeDev:'Responsive Web Development (HTML5/JSON/REST)',tech:'Flask',quoteStatus: "open",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
view quote 80% working
</commit_message>
<xml_diff>
--- a/drafts/CRM-schema.xlsx
+++ b/drafts/CRM-schema.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="31580" yWindow="1540" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Field Names" sheetId="1" r:id="rId1"/>
-    <sheet name="Schema Layout" sheetId="2" r:id="rId2"/>
-    <sheet name="Document Data" sheetId="3" r:id="rId3"/>
-    <sheet name="JSON" sheetId="4" r:id="rId4"/>
-    <sheet name="variables" sheetId="8" r:id="rId5"/>
-    <sheet name="Form" sheetId="9" r:id="rId6"/>
+    <sheet name="Document Data" sheetId="3" r:id="rId2"/>
+    <sheet name="JSON" sheetId="4" r:id="rId3"/>
+    <sheet name="variables" sheetId="8" r:id="rId4"/>
+    <sheet name="Form" sheetId="9" r:id="rId5"/>
+    <sheet name="Schema Layout" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Field Names'!$A$1:$I$23</definedName>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="252">
   <si>
     <t>Your name, please? *</t>
   </si>
@@ -472,36 +472,6 @@
     <t xml:space="preserve"> "sending the standard response",</t>
   </si>
   <si>
-    <t xml:space="preserve"> "1",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "4",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "5",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "6",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "7",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "8",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "9",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "10",</t>
-  </si>
-  <si>
     <t>{{</t>
   </si>
   <si>
@@ -889,42 +859,6 @@
   </si>
   <si>
     <t>"),</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "11",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "12",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "13",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "14",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "15",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "16",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "17",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "18",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "19",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "20",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "21",</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "22",</t>
   </si>
   <si>
     <t>"Mr Drudge",</t>
@@ -2104,7 +2038,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="57" customHeight="1" x14ac:dyDescent="0"/>
@@ -2164,7 +2098,7 @@
         <v>115</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
@@ -2215,7 +2149,7 @@
         <v>115</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -2343,7 +2277,7 @@
         <v>115</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C12" t="s">
         <v>49</v>
@@ -2363,7 +2297,7 @@
         <v>115</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>37</v>
@@ -2450,7 +2384,7 @@
         <v>115</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>37</v>
@@ -2548,7 +2482,7 @@
         <v>116</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>37</v>
@@ -2593,45 +2527,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:AJ22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ22"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2720,71 +2619,71 @@
       <c r="A2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>268</v>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2">
+        <v>9</v>
+      </c>
+      <c r="K2" s="2">
+        <v>10</v>
+      </c>
+      <c r="L2" s="2">
+        <v>11</v>
+      </c>
+      <c r="M2" s="2">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2">
+        <v>13</v>
+      </c>
+      <c r="O2" s="2">
+        <v>14</v>
+      </c>
+      <c r="P2" s="2">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>16</v>
+      </c>
+      <c r="R2" s="2">
+        <v>17</v>
+      </c>
+      <c r="S2" s="2">
+        <v>18</v>
+      </c>
+      <c r="T2" s="2">
+        <v>19</v>
+      </c>
+      <c r="U2" s="2">
+        <v>20</v>
+      </c>
+      <c r="V2" s="2">
+        <v>21</v>
+      </c>
+      <c r="W2" s="2">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:36" ht="31">
@@ -2801,13 +2700,13 @@
         <v>54</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>53</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>97</v>
@@ -2819,13 +2718,13 @@
         <v>54</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>97</v>
@@ -2837,13 +2736,13 @@
         <v>54</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>53</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>97</v>
@@ -2855,7 +2754,7 @@
         <v>54</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="46">
@@ -3644,46 +3543,46 @@
         <v>102</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>79</v>
@@ -3715,107 +3614,107 @@
         <v>94</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="V16" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="X16" s="3"/>
       <c r="Y16" s="2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="AB16" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="AC16" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="AD16" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="AE16" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="AF16" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="AG16" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="AH16" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="AI16" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="AJ16" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="91">
@@ -3968,13 +3867,13 @@
         <v>123</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>123</v>
@@ -4269,12 +4168,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q6" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="T65" sqref="T65"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="66.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4372,91 +4271,91 @@
     <row r="2" spans="1:22">
       <c r="A2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!B2,"',")</f>
-        <v>quoteId:' "1",',</v>
+        <v>quoteId:'1',</v>
       </c>
       <c r="B2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!C2,"',")</f>
-        <v>quoteId:' "2",',</v>
+        <v>quoteId:'2',</v>
       </c>
       <c r="C2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!D2,"',")</f>
-        <v>quoteId:' "3",',</v>
+        <v>quoteId:'3',</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!E2,"',")</f>
-        <v>quoteId:' "4",',</v>
+        <v>quoteId:'4',</v>
       </c>
       <c r="E2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!F2,"',")</f>
-        <v>quoteId:' "5",',</v>
+        <v>quoteId:'5',</v>
       </c>
       <c r="F2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!G2,"',")</f>
-        <v>quoteId:' "6",',</v>
+        <v>quoteId:'6',</v>
       </c>
       <c r="G2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!H2,"',")</f>
-        <v>quoteId:' "7",',</v>
+        <v>quoteId:'7',</v>
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!I2,"',")</f>
-        <v>quoteId:' "8",',</v>
+        <v>quoteId:'8',</v>
       </c>
       <c r="I2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!J2,"',")</f>
-        <v>quoteId:' "9",',</v>
+        <v>quoteId:'9',</v>
       </c>
       <c r="J2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!K2,"',")</f>
-        <v>quoteId:' "10",',</v>
+        <v>quoteId:'10',</v>
       </c>
       <c r="K2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!L2,"',")</f>
-        <v>quoteId:' "11",',</v>
+        <v>quoteId:'11',</v>
       </c>
       <c r="L2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!M2,"',")</f>
-        <v>quoteId:' "12",',</v>
+        <v>quoteId:'12',</v>
       </c>
       <c r="M2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!N2,"',")</f>
-        <v>quoteId:' "13",',</v>
+        <v>quoteId:'13',</v>
       </c>
       <c r="N2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!O2,"',")</f>
-        <v>quoteId:' "14",',</v>
+        <v>quoteId:'14',</v>
       </c>
       <c r="O2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!P2,"',")</f>
-        <v>quoteId:' "15",',</v>
+        <v>quoteId:'15',</v>
       </c>
       <c r="P2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!Q2,"',")</f>
-        <v>quoteId:' "16",',</v>
+        <v>quoteId:'16',</v>
       </c>
       <c r="Q2" t="str">
         <f>CONCATENATE('Document Data'!$A2,"'",'Document Data'!R2,"',")</f>
-        <v>quoteId:' "17",',</v>
+        <v>quoteId:'17',</v>
       </c>
       <c r="R2" t="str">
         <f>CONCATENATE('Document Data'!$A2,'Document Data'!S2)</f>
-        <v>quoteId: "18",</v>
+        <v>quoteId:18</v>
       </c>
       <c r="S2" t="str">
         <f>CONCATENATE('Document Data'!$A2,'Document Data'!T2)</f>
-        <v>quoteId: "19",</v>
+        <v>quoteId:19</v>
       </c>
       <c r="T2" t="str">
         <f>CONCATENATE('Document Data'!$A2,'Document Data'!U2)</f>
-        <v>quoteId: "20",</v>
+        <v>quoteId:20</v>
       </c>
       <c r="U2" t="str">
         <f>CONCATENATE('Document Data'!$A2,'Document Data'!V2)</f>
-        <v>quoteId: "21",</v>
+        <v>quoteId:21</v>
       </c>
       <c r="V2" t="str">
         <f>CONCATENATE('Document Data'!$A2,'Document Data'!W2)</f>
-        <v>quoteId: "22",</v>
+        <v>quoteId:22</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -6262,91 +6161,91 @@
     <row r="27" spans="1:22" ht="272" customHeight="1">
       <c r="A27" s="13" t="str">
         <f>CONCATENATE(A1,A2,A3,A4,A5,A6,A7,A8,A9,A10,A11,A12,A13,A14,A15,A16,A17,A18,A19,A20,A21,A22)</f>
-        <v>coll.insert({quoteId:' "1",',name: "Mr. Simpson",email: "ciaran.quinlan@gmail.com",phone: "0868090777",rankQuality: "Low",rankTime: "Medium",rankCost: "High",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "4000",brief: "Becoming a fullstack web developer requires you to cover a lot of skills. For beginners it’s often not easy to find the right learning path and to gain quick result. At first sight it might be overwhelming to understand what you need to learn and how everything fits together at the end..",typeDev:'Responsive Web Development (HTML5/JSON/REST)',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'1',name: "Mr. Simpson",email: "ciaran.quinlan@gmail.com",phone: "0868090777",rankQuality: "Low",rankTime: "Medium",rankCost: "High",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "4000",brief: "Becoming a fullstack web developer requires you to cover a lot of skills. For beginners it’s often not easy to find the right learning path and to gain quick result. At first sight it might be overwhelming to understand what you need to learn and how everything fits together at the end..",typeDev:'Responsive Web Development (HTML5/JSON/REST)',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="B27" s="13" t="str">
         <f>CONCATENATE(B1,B2,B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19,B20,B21,B22)</f>
-        <v>coll.insert({quoteId:' "2",',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime:"Low",rankCost: "Medium",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "5000",brief: "Becoming a fullstack web developer requires you to cover a lot of skills. For beginners it’s often not easy to find the right learning path and to gain quick result. At first sight it might be overwhelming to understand what you need to learn and how everything fits together at the end..",typeDev:'Native Mobile Application (iOS)',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Leo ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'2',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime:"Low",rankCost: "Medium",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "5000",brief: "Becoming a fullstack web developer requires you to cover a lot of skills. For beginners it’s often not easy to find the right learning path and to gain quick result. At first sight it might be overwhelming to understand what you need to learn and how everything fits together at the end..",typeDev:'Native Mobile Application (iOS)',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Leo ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="C27" s="13" t="str">
         <f t="shared" ref="C27:V27" si="0">CONCATENATE(C1,C2,C3,C4,C5,C6,C7,C8,C9,C10,C11,C12,C13,C14,C15,C16,C17,C18,C19,C20,C21,C22)</f>
-        <v>coll.insert({quoteId:' "3",',name: "Mr. Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "High",rankTime: "Medium",rankCost:"Low",levelQuality:"Jumbo Jet",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This post will give you an overview of technologies you may consider to learn for being a fullstack developer in 2019 and beyond. We’ll start to take a look at the foundation and programming languages and then move forward to more advanced topics like frameworks and additional tools..",typeDev:'E-Commerce Web Development',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Mike ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'3',name: "Mr. Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "High",rankTime: "Medium",rankCost:"Low",levelQuality:"Jumbo Jet",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This post will give you an overview of technologies you may consider to learn for being a fullstack developer in 2019 and beyond. We’ll start to take a look at the foundation and programming languages and then move forward to more advanced topics like frameworks and additional tools..",typeDev:'E-Commerce Web Development',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Mike ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="D27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "4",',name: "Mr Drudge",email:"random@email.com",phone: "0868090777",rankQuality:  "High",rankTime: "High",rankCost: "Medium",levelQuality:"Space Shuttle",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "4000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Database Architecture and Design',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Mary ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'4',name: "Mr Drudge",email:"random@email.com",phone: "0868090777",rankQuality:  "High",rankTime: "High",rankCost: "Medium",levelQuality:"Space Shuttle",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "4000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Database Architecture and Design',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Mary ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="E27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "5",',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality: "Low",rankTime: "Medium",rankCost: "High",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "5000",brief: "this is the detailed brief",typeDev:'Bespoke Software Platform',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'5',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality: "Low",rankTime: "Medium",rankCost: "High",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "5000",brief: "this is the detailed brief",typeDev:'Bespoke Software Platform',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="F27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "6",',name: "Mr. Alan Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime:"Low",rankCost: "Medium",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "Becoming a fullstack web developer requires you to cover a lot of skills. For beginners it’s often not easy to find the right learning path and to gain quick result. At first sight it might be overwhelming to understand what you need to learn and how everything fits together at the end..",typeDev:'Other:',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'6',name: "Mr. Alan Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime:"Low",rankCost: "Medium",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "Becoming a fullstack web developer requires you to cover a lot of skills. For beginners it’s often not easy to find the right learning path and to gain quick result. At first sight it might be overwhelming to understand what you need to learn and how everything fits together at the end..",typeDev:'Other:',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="G27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "7",',name: "Mr. Simpson",email:"random@email.com",phone: "0868090777",rankQuality:  "High",rankTime: "Medium",rankCost:"Low",levelQuality:"Jumbo Jet",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "4000",brief: "This post will give you an overview of technologies you may consider to learn for being a fullstack developer in 2019 and beyond. We’ll start to take a look at the foundation and programming languages and then move forward to more advanced topics like frameworks and additional tools..",typeDev:'Responsive Web Development (HTML5/JSON/REST)',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'7',name: "Mr. Simpson",email:"random@email.com",phone: "0868090777",rankQuality:  "High",rankTime: "Medium",rankCost:"Low",levelQuality:"Jumbo Jet",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "4000",brief: "This post will give you an overview of technologies you may consider to learn for being a fullstack developer in 2019 and beyond. We’ll start to take a look at the foundation and programming languages and then move forward to more advanced topics like frameworks and additional tools..",typeDev:'Responsive Web Development (HTML5/JSON/REST)',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="H27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "8",',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "High",rankTime: "High",rankCost: "Medium",levelQuality:"Space Shuttle",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "5000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Native Mobile Application (iOS)',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'8',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "High",rankTime: "High",rankCost: "Medium",levelQuality:"Space Shuttle",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "5000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Native Mobile Application (iOS)',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="I27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "9",',name: "Mr. Ross",email:"random@email.com",phone: "0868090777",rankQuality: "Low",rankTime:"Low",rankCost: "High",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "this is the detailed brief",typeDev:'E-Commerce Web Development',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'9',name: "Mr. Ross",email:"random@email.com",phone: "0868090777",rankQuality: "Low",rankTime:"Low",rankCost: "High",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "this is the detailed brief",typeDev:'E-Commerce Web Development',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="J27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "10",',name: "Mr Drudge",email:"random@email.com",phone: "0868090777",rankQuality: "Low",rankTime: "Medium",rankCost:"Low",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "4000",brief: "Becoming a fullstack web developer requires you to cover a lot of skills. For beginners it’s often not easy to find the right learning path and to gain quick result. At first sight it might be overwhelming to understand what you need to learn and how everything fits together at the end..",typeDev:'Database Architecture and Design',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'10',name: "Mr Drudge",email:"random@email.com",phone: "0868090777",rankQuality: "Low",rankTime: "Medium",rankCost:"Low",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "4000",brief: "Becoming a fullstack web developer requires you to cover a lot of skills. For beginners it’s often not easy to find the right learning path and to gain quick result. At first sight it might be overwhelming to understand what you need to learn and how everything fits together at the end..",typeDev:'Database Architecture and Design',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="K27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "11",',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Jumbo Jet",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "5000",brief: "This post will give you an overview of technologies you may consider to learn for being a fullstack developer in 2019 and beyond. We’ll start to take a look at the foundation and programming languages and then move forward to more advanced topics like frameworks and additional tools..",typeDev:'Bespoke Software Platform',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'11',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Jumbo Jet",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "5000",brief: "This post will give you an overview of technologies you may consider to learn for being a fullstack developer in 2019 and beyond. We’ll start to take a look at the foundation and programming languages and then move forward to more advanced topics like frameworks and additional tools..",typeDev:'Bespoke Software Platform',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="L27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "12",',name: "Mr. Alan Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Space Shuttle",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Other:',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'12',name: "Mr. Alan Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Space Shuttle",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Other:',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="M27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "13",',name: "Mr. Simpson",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Bespoke Software Platform',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'13',name: "Mr. Simpson",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Bespoke Software Platform',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="N27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "14",',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Other:',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'14',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Other:',tech:["Flask", "Django", "NoSql","HTML","CSS","MongoDB","Magento","Python"],quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="O27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "15",',name: "Mr. Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Jumbo Jet",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Responsive Web Development (HTML5/JSON/REST)',tech:'HTML5',quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'15',name: "Mr. Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Jumbo Jet",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Responsive Web Development (HTML5/JSON/REST)',tech:'HTML5',quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="P27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "16",',name: "Mr Drudge",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Space Shuttle",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Native Mobile Application (iOS)',tech:'HTML5',quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'16',name: "Mr Drudge",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Space Shuttle",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Native Mobile Application (iOS)',tech:'HTML5',quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="Q27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId:' "17",',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Bespoke Software Platform',tech:'SQL',quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:'17',name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Bespoke Software Platform',tech:'SQL',quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="R27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId: "18",name: "Mr. Alan Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Other:',tech:'Flask',quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:18name: "Mr. Alan Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Other:',tech:'Flask',quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="S27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId: "19",name: "Mr. Simpson",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Jumbo Jet",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Responsive Web Development (HTML5/JSON/REST)',tech:'Django',quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:19name: "Mr. Simpson",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Jumbo Jet",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Responsive Web Development (HTML5/JSON/REST)',tech:'Django',quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="T27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId: "20",name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Space Shuttle",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Native Mobile Application (iOS)',tech:'NoSQL',quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:20name: "Mr. Smith",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Space Shuttle",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Native Mobile Application (iOS)',tech:'NoSQL',quoteStatus: "CLOSED",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="U27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId: "21",name: "Mr. Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'E-Commerce Web Development',tech:'Python',quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:21name: "Mr. Ross",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Bike",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'E-Commerce Web Development',tech:'Python',quoteStatus: "PENDING",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
       <c r="V27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>coll.insert({quoteId: "22",name: "Mr Drudge",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Database Architecture and Design',tech:'JavaScript',quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
+        <v>coll.insert({quoteId:22name: "Mr Drudge",email:"random@email.com",phone: "0868090777",rankQuality:  "Medium",rankTime: "High",rankCost: "Medium",levelQuality:"Car",expectedDate: "01/09/2019",liveDate: "01/09/2019",budget: "10000",brief: "This list will provide guidance to find your path through the web development jungle in 2019. Together with a short description of the relevant topics this post contains link to great learning resources so that you can start quickly to expand your skill-set.",typeDev:'Database Architecture and Design',tech:'JavaScript',quoteStatus: "OPEN",quoteDetails: "send me a quote that will meet my requirements",quoteResponse: "sending the standard response",assignedTo: "Joe ryan",quoteCost:"50000",quoteNeeds: "It needs this and that and a whole lot more",});</v>
       </c>
     </row>
   </sheetData>
@@ -6360,7 +6259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -6394,21 +6293,21 @@
         <v>quoteId:</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D2" s="14" t="str">
         <f>A2</f>
         <v>quote</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F2" t="str">
         <f>LEFT(B2,LEN(B2)-1)</f>
         <v>quoteId</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE(C2,D2,E2,F2,G2)</f>
@@ -6425,21 +6324,21 @@
         <v>name:</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D3" s="14" t="str">
         <f t="shared" ref="D3:D23" si="0">A3</f>
         <v>quote</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F23" si="1">LEFT(B3,LEN(B3)-1)</f>
         <v>name</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H23" si="2">CONCATENATE(C3,D3,E3,F3,G3)</f>
@@ -6456,21 +6355,21 @@
         <v>email:</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D4" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
         <v>email</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="2"/>
@@ -6487,21 +6386,21 @@
         <v>phone:</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D5" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
         <v>phone</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="2"/>
@@ -6518,21 +6417,21 @@
         <v>rankQuality:</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D6" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
         <v>rankQuality</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="2"/>
@@ -6549,21 +6448,21 @@
         <v>rankTime:</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D7" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
         <v>rankTime</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="2"/>
@@ -6580,21 +6479,21 @@
         <v>rankCost:</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D8" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
         <v>rankCost</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="2"/>
@@ -6611,21 +6510,21 @@
         <v>levelQuality:</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D9" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
         <v>levelQuality</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="2"/>
@@ -6642,21 +6541,21 @@
         <v>expectedDate:</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D10" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
         <v>expectedDate</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="2"/>
@@ -6673,21 +6572,21 @@
         <v>liveDate:</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D11" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
         <v>liveDate</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="2"/>
@@ -6704,21 +6603,21 @@
         <v>budget:</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D12" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
         <v>budget</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="2"/>
@@ -6735,21 +6634,21 @@
         <v>brief:</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D13" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
         <v>brief</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="2"/>
@@ -6766,21 +6665,21 @@
         <v>typeDev:</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D14" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
         <v>typeDev</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="2"/>
@@ -6797,21 +6696,21 @@
         <v>tech:</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D15" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
         <v>tech</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="2"/>
@@ -6828,21 +6727,21 @@
         <v>quoteStatus:</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D16" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
         <v>quoteStatus</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="2"/>
@@ -6859,21 +6758,21 @@
         <v>quoteDetails:</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D17" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
         <v>quoteDetails</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="2"/>
@@ -6890,21 +6789,21 @@
         <v>quoteResponse:</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D18" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
         <v>quoteResponse</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="2"/>
@@ -6921,21 +6820,21 @@
         <v>assignedTo:</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D19" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
         <v>assignedTo</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="2"/>
@@ -6952,21 +6851,21 @@
         <v>quoteCost:</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D20" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
         <v>quoteCost</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="2"/>
@@ -6983,21 +6882,21 @@
         <v>quoteNeeds:</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D21" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quote</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
         <v>quoteNeeds</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="2"/>
@@ -7014,21 +6913,21 @@
         <v>quoteStatus:</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D22" s="14" t="str">
         <f t="shared" si="0"/>
         <v>status</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
         <v>quoteStatus</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="2"/>
@@ -7045,21 +6944,21 @@
         <v>quoteId:</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D23" s="14" t="str">
         <f t="shared" si="0"/>
         <v>quotenumber</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
         <v>quoteId</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="2"/>
@@ -7077,7 +6976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA24"/>
   <sheetViews>
@@ -7109,55 +7008,55 @@
   <sheetData>
     <row r="1" spans="1:27" s="15" customFormat="1" ht="16">
       <c r="G1" s="15" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="J1" s="15" t="str">
         <f>H1</f>
         <v>quote_phone</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="L1" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="M1" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="P1" s="17" t="s">
-        <v>168</v>
-      </c>
       <c r="Q1" s="15" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="S1" s="15" t="str">
         <f>H1</f>
         <v>quote_phone</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="U1" s="15" t="str">
         <f>M1</f>
         <v>Your Phone Number</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="W1" s="18" t="str">
         <f>CONCATENATE(G1,H1,I1,J1,K1,L1,M1,N1,O1,P1,Q1,R1,S1,T1,U1,V1)</f>
@@ -7187,71 +7086,71 @@
         <v>"quoteId" : request.form.get("quote_id"),</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E4" t="str">
         <f>H4</f>
         <v>quote_id</v>
       </c>
       <c r="F4" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J4" s="15" t="str">
         <f t="shared" ref="J4:J23" si="0">H4</f>
         <v>quote_id</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P4" s="19" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="Q4" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R4" s="15" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="S4" s="15" t="str">
         <f t="shared" ref="S4" si="1">H4</f>
         <v>quote_id</v>
       </c>
       <c r="T4" s="15" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="U4" s="15" t="str">
         <f t="shared" ref="U4" si="2">M4</f>
         <v>Quote Id</v>
       </c>
       <c r="V4" s="15" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="W4" s="18" t="str">
         <f t="shared" ref="W4:W24" si="3">CONCATENATE(G4,H4,I4,J4,K4,L4,M4,N4,O4,P4,Q4,R4,S4,T4,U4,V4)</f>
@@ -7264,54 +7163,54 @@
         <v>"name" : request.form.get("quote_name"),</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" ref="E5:E23" si="4">H5</f>
         <v>quote_name</v>
       </c>
       <c r="F5" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J5" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_name</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O5" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P5" s="19" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="Q5" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R5" s="15"/>
       <c r="S5" s="15"/>
@@ -7329,54 +7228,54 @@
         <v>"email" : request.form.get("quote_email"),</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="4"/>
         <v>quote_email</v>
       </c>
       <c r="F6" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J6" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_email</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P6" s="19" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R6" s="15"/>
       <c r="S6" s="15"/>
@@ -7394,54 +7293,54 @@
         <v>"phone" : request.form.get("quote_phone"),</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="4"/>
         <v>quote_phone</v>
       </c>
       <c r="F7" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J7" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_phone</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O7" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P7" s="19" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R7" s="15"/>
       <c r="S7" s="15"/>
@@ -7459,54 +7358,54 @@
         <v>"rankQuality" : request.form.get("quote_rankquality"),</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="4"/>
         <v>quote_rankquality</v>
       </c>
       <c r="F8" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J8" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_rankquality</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O8" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P8" s="19" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
@@ -7524,54 +7423,54 @@
         <v>"rankTime" : request.form.get("quote_ranktime"),</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="4"/>
         <v>quote_ranktime</v>
       </c>
       <c r="F9" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J9" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_ranktime</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O9" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R9" s="15"/>
       <c r="S9" s="15"/>
@@ -7589,54 +7488,54 @@
         <v>"rankCost" : request.form.get("quote_rankcost"),</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="4"/>
         <v>quote_rankcost</v>
       </c>
       <c r="F10" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J10" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_rankcost</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O10" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R10" s="15"/>
       <c r="S10" s="15"/>
@@ -7654,54 +7553,54 @@
         <v>"levelQuality" : request.form.get("quote_expectedquality"),</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="4"/>
         <v>quote_expectedquality</v>
       </c>
       <c r="F11" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J11" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_expectedquality</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O11" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="Q11" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R11" s="15"/>
       <c r="S11" s="15"/>
@@ -7719,54 +7618,54 @@
         <v>"expectedDate" : request.form.get("quote_expecteddate"),</v>
       </c>
       <c r="B12" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>244</v>
-      </c>
       <c r="D12" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="4"/>
         <v>quote_expecteddate</v>
       </c>
       <c r="F12" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J12" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_expecteddate</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O12" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="Q12" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R12" s="15"/>
       <c r="S12" s="15"/>
@@ -7784,54 +7683,54 @@
         <v>"liveDate" : request.form.get("quote_livedate"),</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C13" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>245</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>255</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="4"/>
         <v>quote_livedate</v>
       </c>
       <c r="F13" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J13" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_livedate</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="N13" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="O13" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="P13" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="O13" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="P13" s="19" t="s">
-        <v>174</v>
-      </c>
       <c r="Q13" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R13" s="15"/>
       <c r="S13" s="15"/>
@@ -7849,54 +7748,54 @@
         <v>"budget" : request.form.get("quote_budget "),</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">quote_budget </v>
       </c>
       <c r="F14" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J14" s="15" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">quote_budget </v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="N14" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O14" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="Q14" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R14" s="15"/>
       <c r="S14" s="15"/>
@@ -7914,54 +7813,54 @@
         <v>"brief" : request.form.get("quote_brief"),</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="4"/>
         <v>quote_brief</v>
       </c>
       <c r="F15" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J15" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_brief</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="N15" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O15" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="Q15" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R15" s="15"/>
       <c r="S15" s="15"/>
@@ -7979,54 +7878,54 @@
         <v>"typeDev" : request.form.get("quote_typedev"),</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="4"/>
         <v>quote_typedev</v>
       </c>
       <c r="F16" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J16" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_typedev</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="N16" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O16" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="Q16" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R16" s="15"/>
       <c r="S16" s="15"/>
@@ -8044,54 +7943,54 @@
         <v>"tech" : request.form.get("quote_tech"),</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="4"/>
         <v>quote_tech</v>
       </c>
       <c r="F17" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J17" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_tech</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M17" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="O17" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="P17" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q17" s="15" t="s">
         <v>222</v>
-      </c>
-      <c r="N17" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="O17" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="P17" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q17" s="15" t="s">
-        <v>232</v>
       </c>
       <c r="R17" s="15"/>
       <c r="S17" s="15"/>
@@ -8109,54 +8008,54 @@
         <v>"quoteStatus" : request.form.get("quote_quotestatus"),</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="4"/>
         <v>quote_quotestatus</v>
       </c>
       <c r="F18" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J18" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_quotestatus</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="N18" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O18" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="Q18" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R18" s="15"/>
       <c r="S18" s="15"/>
@@ -8174,54 +8073,54 @@
         <v>"quoteDetails" : request.form.get("quote_details"),</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="4"/>
         <v>quote_details</v>
       </c>
       <c r="F19" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J19" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_details</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M19" s="17" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="N19" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O19" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="Q19" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R19" s="15"/>
       <c r="S19" s="15"/>
@@ -8239,54 +8138,54 @@
         <v>"quoteResponse" : request.form.get("quote_response"),</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="4"/>
         <v>quote_response</v>
       </c>
       <c r="F20" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J20" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_response</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="N20" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O20" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="Q20" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R20" s="15"/>
       <c r="S20" s="15"/>
@@ -8304,54 +8203,54 @@
         <v>"assignedTo" : request.form.get("quote_person"),</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="4"/>
         <v>quote_person</v>
       </c>
       <c r="F21" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J21" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_person</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M21" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="O21" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="N21" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="O21" s="15" t="s">
-        <v>229</v>
-      </c>
       <c r="P21" s="19" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="Q21" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R21" s="15"/>
       <c r="S21" s="15"/>
@@ -8369,54 +8268,54 @@
         <v>"quoteCost" : request.form.get("quote_cost"),</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="4"/>
         <v>quote_cost</v>
       </c>
       <c r="F22" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J22" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_cost</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L22" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O22" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="Q22" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R22" s="15"/>
       <c r="S22" s="15"/>
@@ -8434,54 +8333,54 @@
         <v>"quoteNeeds" : request.form.get("quote_needs"),</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="4"/>
         <v>quote_needs</v>
       </c>
       <c r="F23" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J23" s="15" t="str">
         <f t="shared" si="0"/>
         <v>quote_needs</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O23" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="Q23" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="R23" s="15"/>
       <c r="S23" s="15"/>
@@ -8514,4 +8413,39 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>